<commit_message>
improve default values in vendors mapping
</commit_message>
<xml_diff>
--- a/models/test_data_IZ_to_IZ.xlsx
+++ b/models/test_data_IZ_to_IZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaphaëlRey\PycharmProjects\iz_to_iz_transfer\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3117C9-0FA0-4615-BC72-3FBC288F11A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1228756B-6028-43C8-98C6-D4E1F24AB24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="800" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="11370" tabRatio="800" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Loans" sheetId="10" r:id="rId6"/>
     <sheet name="Requests" sheetId="11" r:id="rId7"/>
     <sheet name="Locations_mapping" sheetId="3" r:id="rId8"/>
-    <sheet name="Item_policies_mapping" sheetId="5" r:id="rId9"/>
+    <sheet name="Funds_mapping" sheetId="12" r:id="rId9"/>
     <sheet name="Vendors_mapping" sheetId="7" r:id="rId10"/>
     <sheet name="data_validation" sheetId="4" state="hidden" r:id="rId11"/>
   </sheets>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
   <si>
     <t>Barcode</t>
   </si>
@@ -200,15 +200,6 @@
     <t>*DEFAULT*</t>
   </si>
   <si>
-    <t>Source item policy code</t>
-  </si>
-  <si>
-    <t>Destination item policy code</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
     <t>Yes / No</t>
   </si>
   <si>
@@ -245,39 +236,15 @@
     <t>9911787970105504</t>
   </si>
   <si>
-    <t>Vendor code src</t>
-  </si>
-  <si>
-    <t>Vendor account src</t>
-  </si>
-  <si>
-    <t>Vendor code dest</t>
-  </si>
-  <si>
-    <t>Vendor account dest</t>
-  </si>
-  <si>
     <t>ABC_vendor</t>
   </si>
   <si>
     <t>12345</t>
   </si>
   <si>
-    <t>LIB_ABC_Vendor</t>
-  </si>
-  <si>
-    <t>012345</t>
-  </si>
-  <si>
     <t>provenance</t>
   </si>
   <si>
-    <t>temp_loacation, temp_library, in_temp_location</t>
-  </si>
-  <si>
-    <t>PoLine</t>
-  </si>
-  <si>
     <t>pattern_type</t>
   </si>
   <si>
@@ -290,27 +257,12 @@
     <t>statistics_note_3</t>
   </si>
   <si>
-    <t>Always</t>
-  </si>
-  <si>
-    <t>Never</t>
-  </si>
-  <si>
-    <t>When</t>
-  </si>
-  <si>
-    <t>Keep the following item fields</t>
-  </si>
-  <si>
     <t>Version</t>
   </si>
   <si>
     <t>5.0</t>
   </si>
   <si>
-    <t>No error</t>
-  </si>
-  <si>
     <t>SLSP: Transfer IZ to IZ</t>
   </si>
   <si>
@@ -318,6 +270,117 @@
   </si>
   <si>
     <t>In source items</t>
+  </si>
+  <si>
+    <t>Library code source</t>
+  </si>
+  <si>
+    <t>Library code destination</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Keep fields</t>
+  </si>
+  <si>
+    <t>Always delete</t>
+  </si>
+  <si>
+    <t>Delete if error</t>
+  </si>
+  <si>
+    <t>Never delete</t>
+  </si>
+  <si>
+    <t>Delete the following item fields</t>
+  </si>
+  <si>
+    <t>The "provenance" field contains configured values in a table. The same values must be configured in the destination IZ to avoid errors.</t>
+  </si>
+  <si>
+    <t>In order to keep this information, the destination institution must have the same values and codes.</t>
+  </si>
+  <si>
+    <t>The same PoLine number is never possible. The decision to keep the PoLine field will prevent the copying of any item with PoLine information. When migrating a PoLine, the system will create a new PoLine with a different number.</t>
+  </si>
+  <si>
+    <t>If this field contains erroneous data according to the holding, it will prevent the data from being copied in the destination.</t>
+  </si>
+  <si>
+    <t>Statistics note fields values are configured in a table. The same values must be configured in the destination IZ to avoid errors.</t>
+  </si>
+  <si>
+    <t>po_line</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Not used in the process</t>
+  </si>
+  <si>
+    <t>Used to validate the form</t>
+  </si>
+  <si>
+    <t>PO Line Reference</t>
+  </si>
+  <si>
+    <t>MMS Id</t>
+  </si>
+  <si>
+    <t>Holdings ID</t>
+  </si>
+  <si>
+    <t>Physical Item Id</t>
+  </si>
+  <si>
+    <t>9972798270405504</t>
+  </si>
+  <si>
+    <t>22434853660005504</t>
+  </si>
+  <si>
+    <t>23454312290005504</t>
+  </si>
+  <si>
+    <t>23454312280005504</t>
+  </si>
+  <si>
+    <t>23443623250005504</t>
+  </si>
+  <si>
+    <t>POL-UBS-2025-167396</t>
+  </si>
+  <si>
+    <t>Fundforall</t>
+  </si>
+  <si>
+    <t>A100-1043</t>
+  </si>
+  <si>
+    <t>000007023</t>
+  </si>
+  <si>
+    <t>Source vendor code</t>
+  </si>
+  <si>
+    <t>Source vendor account</t>
+  </si>
+  <si>
+    <t>Destination vendor code</t>
+  </si>
+  <si>
+    <t>Destination vendor account</t>
+  </si>
+  <si>
+    <t>Source fund code</t>
+  </si>
+  <si>
+    <t>Destination fund code</t>
+  </si>
+  <si>
+    <t>temp_location, temp_library, in_temp_location</t>
   </si>
 </sst>
 </file>
@@ -386,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -406,6 +469,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,22 +787,23 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="25.08984375" customWidth="1"/>
-    <col min="2" max="3" width="13.6328125" customWidth="1"/>
-    <col min="4" max="4" width="52.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="62.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="36">
       <c r="A1" s="9" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -746,121 +811,179 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="C4" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>70</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30.5" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" ht="29">
-      <c r="A10" s="10" t="s">
+    <row r="12" spans="1:4" ht="30.5" customHeight="1">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" ht="29">
+      <c r="A13" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="29">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="29">
+      <c r="A15" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="3" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="46" customHeight="1">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="43.5">
-      <c r="A12" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="D16" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="29">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="3" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="29">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    <row r="20" spans="1:4" ht="29">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -874,25 +997,25 @@
           <x14:formula1>
             <xm:f>data_validation!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
+          <xm:sqref>B10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AD1CBFF3-7A39-414B-8090-527E27A9FEB0}">
           <x14:formula1>
             <xm:f>data_validation!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
+          <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3BA26AD9-284C-4EA0-B5B0-2A9B21BCA870}">
           <x14:formula1>
             <xm:f>data_validation!$A$2:$A$32</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B6</xm:sqref>
+          <xm:sqref>B6:B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{393A7292-E0D0-4C92-A355-7A2CA343F80F}">
           <x14:formula1>
             <xm:f>data_validation!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B11:C17</xm:sqref>
+          <xm:sqref>B14:C20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -905,10 +1028,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -918,34 +1041,59 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>73</v>
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -954,7 +1102,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
@@ -967,31 +1115,27 @@
         <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
@@ -1001,10 +1145,10 @@
         <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1012,7 +1156,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1169,7 +1313,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
@@ -1221,7 +1365,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1232,34 +1376,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1286,7 +1430,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1308,15 +1452,76 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="4" width="20.81640625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1360,7 +1565,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
@@ -1408,44 +1613,51 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206F50D4-37BA-4D0A-9619-E97216BE8408}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED99D418-FB11-4449-B88D-57A5CC883B32}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" style="5" customWidth="1"/>
+    <col min="1" max="2" width="25.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>52</v>
+      <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>53</v>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update clean test data
</commit_message>
<xml_diff>
--- a/models/test_data_IZ_to_IZ.xlsx
+++ b/models/test_data_IZ_to_IZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaphaëlRey\PycharmProjects\iz_to_iz_transfer\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1228756B-6028-43C8-98C6-D4E1F24AB24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACF54B2-1B6B-45FD-99E3-F3061745B368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="11370" tabRatio="800" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="12645" tabRatio="800" activeTab="7" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
   <si>
     <t>Barcode</t>
   </si>
@@ -789,16 +789,16 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.08984375" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" customWidth="1"/>
-    <col min="4" max="4" width="62.7265625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="36">
@@ -869,13 +869,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30.5" customHeight="1">
+    <row r="12" spans="1:4" ht="30.6" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" ht="29">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="10" t="s">
         <v>82</v>
       </c>
@@ -889,7 +889,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29">
+    <row r="14" spans="1:4" ht="45">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -903,7 +903,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="29">
+    <row r="15" spans="1:4" ht="45">
       <c r="A15" s="7" t="s">
         <v>111</v>
       </c>
@@ -917,7 +917,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="46" customHeight="1">
+    <row r="16" spans="1:4" ht="45.95" customHeight="1">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -931,7 +931,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="29">
+    <row r="17" spans="1:4" ht="30">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -945,7 +945,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29">
+    <row r="18" spans="1:4" ht="30">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -959,7 +959,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="29">
+    <row r="19" spans="1:4" ht="30">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -973,7 +973,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="29">
+    <row r="20" spans="1:4" ht="30">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1034,9 +1034,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="20.7265625" style="5" customWidth="1"/>
+    <col min="1" max="4" width="20.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1105,7 +1105,7 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -1316,9 +1316,9 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1368,10 +1368,10 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" customWidth="1"/>
-    <col min="2" max="2" width="20.90625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1423,9 +1423,9 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1458,9 +1458,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="20.81640625" style="5" customWidth="1"/>
+    <col min="1" max="4" width="20.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1534,7 +1534,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1551,7 +1551,7 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1564,13 +1564,13 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="25.81640625" customWidth="1"/>
+    <col min="1" max="4" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1594,8 +1594,12 @@
       <c r="B2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2">
+        <v>610940001</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
@@ -1628,9 +1632,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="25.81640625" customWidth="1"/>
+    <col min="1" max="2" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>